<commit_message>
Added Attendance Model and Attendance API
</commit_message>
<xml_diff>
--- a/TrainerFile.xlsx
+++ b/TrainerFile.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,95 +421,43 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>mskn</v>
+        <v>Dency Patel</v>
       </c>
       <c r="B2" t="str">
-        <v>sai@gmail.com</v>
+        <v>dency.patel@accolitedigital.com</v>
       </c>
       <c r="C2" t="str">
-        <v>65363753</v>
+        <v>7629163826</v>
       </c>
       <c r="D2" t="str">
-        <v>react</v>
+        <v>REACT</v>
       </c>
       <c r="E2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Date:2023-04-24    FromTime:null     ToTime:null
-Date:2023-04-20    FromTime:09:00:00     ToTime:17:00:00</v>
+        <v xml:space="preserve">Date:2023-04-26    FromTime:10:00:00     ToTime:17:00:00
+Date:2023-04-27    FromTime:10:00:00     ToTime:17:00:00</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>Aman</v>
+        <v>Pratyush Singh</v>
       </c>
       <c r="B3" t="str">
-        <v>aman@gmail.com</v>
+        <v>pratyush.singh@accolitedigital.com</v>
       </c>
       <c r="C3" t="str">
-        <v>656537</v>
+        <v>8761826384</v>
       </c>
       <c r="D3" t="str">
-        <v>React</v>
+        <v>SPRING</v>
       </c>
       <c r="E3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Date:2023-04-21    FromTime:09:00:00     ToTime:17:00:00
-Date:2023-04-20    FromTime:09:00:00     ToTime:17:00:00</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4" t="str">
-        <v>viswa</v>
-      </c>
-      <c r="B4" t="str">
-        <v>viswa@gmail.com</v>
-      </c>
-      <c r="C4" t="str">
-        <v>654633</v>
-      </c>
-      <c r="D4" t="str">
-        <v>React</v>
-      </c>
-      <c r="E4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Date:2023-04-22    FromTime:09:00:00     ToTime:13:00:00
-Date:2023-04-22    FromTime:09:00:00     ToTime:17:00:00</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>aakriti</v>
-      </c>
-      <c r="B5" t="str">
-        <v>aakriti@gmail.com</v>
-      </c>
-      <c r="C5" t="str">
-        <v>65863858</v>
-      </c>
-      <c r="D5" t="str">
-        <v>React</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Date:2023-04-20    FromTime:09:00:00     ToTime:17:00:00</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>sai</v>
-      </c>
-      <c r="B6" t="str">
-        <v>sai21@gmail.com</v>
-      </c>
-      <c r="C6" t="str">
-        <v>2345253</v>
-      </c>
-      <c r="D6" t="str">
-        <v>sql</v>
-      </c>
-      <c r="E6" t="str">
-        <v/>
+        <v xml:space="preserve">Date:2023-04-28    FromTime:10:00:00     ToTime:17:00:00
+Date:2023-04-29    FromTime:09:00:00     ToTime:17:00:00</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added annotations for role based authorization to all APIs and fixed the attendance API
</commit_message>
<xml_diff>
--- a/TrainerFile.xlsx
+++ b/TrainerFile.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,48 +416,41 @@
         <v>SKILL</v>
       </c>
       <c r="E1" t="str">
-        <v>AVAILABILITY LIST</v>
+        <v>DATE</v>
+      </c>
+      <c r="F1" t="str">
+        <v>FROM TIME</v>
+      </c>
+      <c r="G1" t="str">
+        <v>TO TIME</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
+    <row r="2">
       <c r="A2" t="str">
-        <v>Dency Patel</v>
+        <v>Pratyush Singh</v>
       </c>
       <c r="B2" t="str">
-        <v>dency.patel@accolitedigital.com</v>
+        <v>pratyush.singh@accolitedigital.com</v>
       </c>
       <c r="C2" t="str">
-        <v>7629163826</v>
+        <v>8761826384</v>
       </c>
       <c r="D2" t="str">
-        <v>REACT</v>
-      </c>
-      <c r="E2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Date:2023-04-26    FromTime:10:00:00     ToTime:17:00:00
-Date:2023-04-27    FromTime:10:00:00     ToTime:17:00:00</v>
-      </c>
-    </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
-        <v>Pratyush Singh</v>
-      </c>
-      <c r="B3" t="str">
-        <v>pratyush.singh@accolitedigital.com</v>
-      </c>
-      <c r="C3" t="str">
-        <v>8761826384</v>
-      </c>
-      <c r="D3" t="str">
         <v>SPRING</v>
       </c>
-      <c r="E3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Date:2023-04-28    FromTime:10:00:00     ToTime:17:00:00
-Date:2023-04-29    FromTime:09:00:00     ToTime:17:00:00</v>
+      <c r="E2" t="str">
+        <v>2023-04-29</v>
+      </c>
+      <c r="F2" t="str">
+        <v>09:00:00</v>
+      </c>
+      <c r="G2" t="str">
+        <v>17:00:00</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>